<commit_message>
Toevoeging uitgaves (bestelling van eerste testpomp)
</commit_message>
<xml_diff>
--- a/Opleverset/Extra documenten/Uitgaves_Floating_Farm.xlsx
+++ b/Opleverset/Extra documenten/Uitgaves_Floating_Farm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Extra documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4131ACA6-A481-4792-A586-4051C0B596BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6B94AE-4713-4BD6-BA8B-075C3C3ACD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{14AEBCC3-6D87-4B1A-9D64-0CD8C4A83626}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Item</t>
   </si>
@@ -48,12 +48,24 @@
   </si>
   <si>
     <t>Houten plaat, prototype 1</t>
+  </si>
+  <si>
+    <t>Mini Waterpomp x1</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>19/09/2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -83,9 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,39 +434,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68DF2FA7-E7C3-4436-AF28-B59F61D87239}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.90625" customWidth="1"/>
     <col min="2" max="2" width="14.36328125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="E2" s="1">
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1">
         <f>SUM(C2:C1048576)</f>
-        <v>5</v>
+        <v>9.370000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>4.37</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>